<commit_message>
Push Mittwoch 11.12.19 ich erstelle ein GUI mit Tkinter. bis jetzt habe ich die aufgaben 1 und 2 erledigt
</commit_message>
<xml_diff>
--- a/Zeitplanung SudoSolve.xlsx
+++ b/Zeitplanung SudoSolve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritzwicki/Sudo_Solve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9902217E-95E7-5448-AF6C-C787CBCA3FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598466AB-829B-9643-902D-7E0AA805D676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="4260" windowWidth="28800" windowHeight="12440" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
   <si>
     <t>Nr.</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>Anforderung #08</t>
-  </si>
-  <si>
-    <t>Anforderung #09</t>
   </si>
   <si>
     <t>Testfälle erstellen</t>
@@ -385,7 +382,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,18 +495,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="49">
     <border>
@@ -1154,7 +1139,7 @@
     </xf>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1451,6 +1436,22 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1481,50 +1482,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1700,19 +1657,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2213,8 +2170,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1"/>
@@ -2335,7 +2292,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="85"/>
       <c r="H3" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -2465,7 +2422,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="22"/>
       <c r="H5" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="6"/>
@@ -2533,88 +2490,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="89" t="s">
+      <c r="C7" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="89"/>
+      <c r="D7" s="93"/>
       <c r="E7" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="90" t="s">
+      <c r="G7" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="94"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="90" t="s">
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="94"/>
+      <c r="R7" s="94"/>
+      <c r="S7" s="94"/>
+      <c r="T7" s="95"/>
+      <c r="U7" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="90"/>
-      <c r="S7" s="90"/>
-      <c r="T7" s="91"/>
-      <c r="U7" s="90" t="s">
+      <c r="V7" s="94"/>
+      <c r="W7" s="94"/>
+      <c r="X7" s="94"/>
+      <c r="Y7" s="94"/>
+      <c r="Z7" s="94"/>
+      <c r="AA7" s="95"/>
+      <c r="AB7" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="V7" s="90"/>
-      <c r="W7" s="90"/>
-      <c r="X7" s="90"/>
-      <c r="Y7" s="90"/>
-      <c r="Z7" s="90"/>
-      <c r="AA7" s="91"/>
-      <c r="AB7" s="92" t="s">
+      <c r="AC7" s="94"/>
+      <c r="AD7" s="94"/>
+      <c r="AE7" s="94"/>
+      <c r="AF7" s="94"/>
+      <c r="AG7" s="94"/>
+      <c r="AH7" s="95"/>
+      <c r="AI7" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="AC7" s="90"/>
-      <c r="AD7" s="90"/>
-      <c r="AE7" s="90"/>
-      <c r="AF7" s="90"/>
-      <c r="AG7" s="90"/>
-      <c r="AH7" s="91"/>
-      <c r="AI7" s="90" t="s">
+      <c r="AJ7" s="94"/>
+      <c r="AK7" s="94"/>
+      <c r="AL7" s="94"/>
+      <c r="AM7" s="94"/>
+      <c r="AN7" s="94"/>
+      <c r="AO7" s="95"/>
+      <c r="AP7" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="AJ7" s="90"/>
-      <c r="AK7" s="90"/>
-      <c r="AL7" s="90"/>
-      <c r="AM7" s="90"/>
-      <c r="AN7" s="90"/>
-      <c r="AO7" s="91"/>
-      <c r="AP7" s="92" t="s">
+      <c r="AQ7" s="94"/>
+      <c r="AR7" s="94"/>
+      <c r="AS7" s="94"/>
+      <c r="AT7" s="94"/>
+      <c r="AU7" s="94"/>
+      <c r="AV7" s="95"/>
+      <c r="AW7" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="AQ7" s="90"/>
-      <c r="AR7" s="90"/>
-      <c r="AS7" s="90"/>
-      <c r="AT7" s="90"/>
-      <c r="AU7" s="90"/>
-      <c r="AV7" s="91"/>
-      <c r="AW7" s="90" t="s">
+      <c r="AX7" s="94"/>
+      <c r="AY7" s="94"/>
+      <c r="AZ7" s="94"/>
+      <c r="BA7" s="94"/>
+      <c r="BB7" s="94"/>
+      <c r="BC7" s="95"/>
+      <c r="BD7" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="AX7" s="90"/>
-      <c r="AY7" s="90"/>
-      <c r="AZ7" s="90"/>
-      <c r="BA7" s="90"/>
-      <c r="BB7" s="90"/>
-      <c r="BC7" s="91"/>
-      <c r="BD7" s="92" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE7" s="90"/>
-      <c r="BF7" s="90"/>
-      <c r="BG7" s="90"/>
-      <c r="BH7" s="90"/>
-      <c r="BI7" s="90"/>
-      <c r="BJ7" s="93"/>
+      <c r="BE7" s="94"/>
+      <c r="BF7" s="94"/>
+      <c r="BG7" s="94"/>
+      <c r="BH7" s="94"/>
+      <c r="BI7" s="94"/>
+      <c r="BJ7" s="97"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1">
       <c r="A8" s="10" t="s">
@@ -2631,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>17</v>
@@ -2815,7 +2772,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2884,14 +2841,14 @@
         <v>12</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="84"/>
       <c r="E10" s="48">
         <v>1</v>
       </c>
       <c r="F10" s="87" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="54"/>
@@ -2916,16 +2873,16 @@
       <c r="AA10" s="58"/>
       <c r="AB10" s="53"/>
       <c r="AC10" s="54"/>
-      <c r="AD10" s="103"/>
-      <c r="AE10" s="55"/>
-      <c r="AF10" s="56"/>
+      <c r="AD10" s="53"/>
+      <c r="AE10" s="54"/>
+      <c r="AF10" s="53"/>
       <c r="AG10" s="57"/>
       <c r="AH10" s="58"/>
       <c r="AI10" s="53"/>
       <c r="AJ10" s="54"/>
-      <c r="AK10" s="55"/>
-      <c r="AL10" s="55"/>
-      <c r="AM10" s="106"/>
+      <c r="AK10" s="54"/>
+      <c r="AL10" s="53"/>
+      <c r="AM10" s="54"/>
       <c r="AN10" s="57"/>
       <c r="AO10" s="58"/>
       <c r="AP10" s="53"/>
@@ -2955,14 +2912,13 @@
         <v>102</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="49">
         <v>3</v>
       </c>
       <c r="D11" s="83">
-        <f>SUM(G11:BJ11)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E11" s="50">
         <v>1</v>
@@ -2972,7 +2928,9 @@
       <c r="H11" s="60"/>
       <c r="I11" s="61"/>
       <c r="J11" s="61"/>
-      <c r="K11" s="63"/>
+      <c r="K11" s="63">
+        <v>4</v>
+      </c>
       <c r="L11" s="62"/>
       <c r="M11" s="58" t="s">
         <v>5</v>
@@ -2995,16 +2953,16 @@
       <c r="AA11" s="58"/>
       <c r="AB11" s="59"/>
       <c r="AC11" s="60"/>
-      <c r="AD11" s="102"/>
-      <c r="AE11" s="61"/>
-      <c r="AF11" s="99"/>
+      <c r="AD11" s="59"/>
+      <c r="AE11" s="60"/>
+      <c r="AF11" s="59"/>
       <c r="AG11" s="57"/>
       <c r="AH11" s="58"/>
       <c r="AI11" s="59"/>
       <c r="AJ11" s="60"/>
-      <c r="AK11" s="61"/>
-      <c r="AL11" s="61"/>
-      <c r="AM11" s="106"/>
+      <c r="AK11" s="60"/>
+      <c r="AL11" s="59"/>
+      <c r="AM11" s="60"/>
       <c r="AN11" s="57"/>
       <c r="AO11" s="58"/>
       <c r="AP11" s="59"/>
@@ -3041,7 +2999,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -3051,7 +3009,9 @@
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="63"/>
+      <c r="K12" s="63">
+        <v>0.5</v>
+      </c>
       <c r="L12" s="57"/>
       <c r="M12" s="58"/>
       <c r="N12" s="59"/>
@@ -3070,16 +3030,16 @@
       <c r="AA12" s="58"/>
       <c r="AB12" s="59"/>
       <c r="AC12" s="60"/>
-      <c r="AD12" s="102"/>
-      <c r="AE12" s="61"/>
-      <c r="AF12" s="99"/>
+      <c r="AD12" s="59"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="59"/>
       <c r="AG12" s="57"/>
       <c r="AH12" s="58"/>
       <c r="AI12" s="59"/>
       <c r="AJ12" s="60"/>
-      <c r="AK12" s="61"/>
-      <c r="AL12" s="61"/>
-      <c r="AM12" s="106"/>
+      <c r="AK12" s="60"/>
+      <c r="AL12" s="59"/>
+      <c r="AM12" s="60"/>
       <c r="AN12" s="57"/>
       <c r="AO12" s="58"/>
       <c r="AP12" s="59"/>
@@ -3109,17 +3069,17 @@
         <v>104</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="50">
         <v>1</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="59"/>
       <c r="H13" s="60"/>
@@ -3144,16 +3104,16 @@
       <c r="AA13" s="67"/>
       <c r="AB13" s="59"/>
       <c r="AC13" s="60"/>
-      <c r="AD13" s="103"/>
-      <c r="AE13" s="55"/>
-      <c r="AF13" s="55"/>
+      <c r="AD13" s="59"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="59"/>
       <c r="AG13" s="66"/>
       <c r="AH13" s="67"/>
       <c r="AI13" s="59"/>
       <c r="AJ13" s="60"/>
-      <c r="AK13" s="55"/>
-      <c r="AL13" s="55"/>
-      <c r="AM13" s="103"/>
+      <c r="AK13" s="60"/>
+      <c r="AL13" s="59"/>
+      <c r="AM13" s="60"/>
       <c r="AN13" s="66"/>
       <c r="AO13" s="67"/>
       <c r="AP13" s="59"/>
@@ -3218,7 +3178,7 @@
       <c r="AA14" s="76"/>
       <c r="AB14" s="77"/>
       <c r="AC14" s="74"/>
-      <c r="AD14" s="104"/>
+      <c r="AD14" s="74"/>
       <c r="AE14" s="74"/>
       <c r="AF14" s="75"/>
       <c r="AG14" s="75"/>
@@ -3227,7 +3187,7 @@
       <c r="AJ14" s="74"/>
       <c r="AK14" s="74"/>
       <c r="AL14" s="74"/>
-      <c r="AM14" s="107"/>
+      <c r="AM14" s="74"/>
       <c r="AN14" s="75"/>
       <c r="AO14" s="76"/>
       <c r="AP14" s="73"/>
@@ -3257,7 +3217,7 @@
         <v>201</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="49">
         <v>7</v>
@@ -3267,13 +3227,13 @@
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
       <c r="I15" s="68"/>
       <c r="J15" s="86"/>
-      <c r="K15" s="99"/>
+      <c r="K15" s="90"/>
       <c r="L15" s="57"/>
       <c r="M15" s="58"/>
       <c r="N15" s="53"/>
@@ -3292,16 +3252,16 @@
       <c r="AA15" s="58"/>
       <c r="AB15" s="53"/>
       <c r="AC15" s="54"/>
-      <c r="AD15" s="103"/>
-      <c r="AE15" s="55"/>
-      <c r="AF15" s="56"/>
+      <c r="AD15" s="53"/>
+      <c r="AE15" s="54"/>
+      <c r="AF15" s="53"/>
       <c r="AG15" s="57"/>
       <c r="AH15" s="58"/>
       <c r="AI15" s="53"/>
       <c r="AJ15" s="54"/>
-      <c r="AK15" s="55"/>
-      <c r="AL15" s="55"/>
-      <c r="AM15" s="106"/>
+      <c r="AK15" s="53"/>
+      <c r="AL15" s="54"/>
+      <c r="AM15" s="53"/>
       <c r="AN15" s="57"/>
       <c r="AO15" s="58"/>
       <c r="AP15" s="53"/>
@@ -3331,7 +3291,7 @@
         <v>202</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="49">
         <v>4</v>
@@ -3351,7 +3311,7 @@
       <c r="M16" s="58"/>
       <c r="N16" s="59"/>
       <c r="O16" s="60"/>
-      <c r="P16" s="98"/>
+      <c r="P16" s="89"/>
       <c r="Q16" s="55"/>
       <c r="R16" s="56"/>
       <c r="S16" s="57"/>
@@ -3365,16 +3325,16 @@
       <c r="AA16" s="58"/>
       <c r="AB16" s="59"/>
       <c r="AC16" s="60"/>
-      <c r="AD16" s="103"/>
-      <c r="AE16" s="55"/>
-      <c r="AF16" s="56"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="60"/>
+      <c r="AF16" s="59"/>
       <c r="AG16" s="57"/>
       <c r="AH16" s="58"/>
       <c r="AI16" s="59"/>
       <c r="AJ16" s="60"/>
-      <c r="AK16" s="55"/>
-      <c r="AL16" s="55"/>
-      <c r="AM16" s="106"/>
+      <c r="AK16" s="59"/>
+      <c r="AL16" s="60"/>
+      <c r="AM16" s="59"/>
       <c r="AN16" s="57"/>
       <c r="AO16" s="58"/>
       <c r="AP16" s="59"/>
@@ -3434,16 +3394,16 @@
       <c r="AA17" s="58"/>
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
-      <c r="AD17" s="103"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="56"/>
+      <c r="AD17" s="69"/>
+      <c r="AE17" s="70"/>
+      <c r="AF17" s="69"/>
       <c r="AG17" s="57"/>
       <c r="AH17" s="58"/>
       <c r="AI17" s="69"/>
       <c r="AJ17" s="70"/>
-      <c r="AK17" s="55"/>
-      <c r="AL17" s="55"/>
-      <c r="AM17" s="106"/>
+      <c r="AK17" s="69"/>
+      <c r="AL17" s="70"/>
+      <c r="AM17" s="69"/>
       <c r="AN17" s="57"/>
       <c r="AO17" s="58"/>
       <c r="AP17" s="69"/>
@@ -3481,7 +3441,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3508,7 +3468,7 @@
       <c r="AA18" s="76"/>
       <c r="AB18" s="77"/>
       <c r="AC18" s="74"/>
-      <c r="AD18" s="104"/>
+      <c r="AD18" s="77"/>
       <c r="AE18" s="74"/>
       <c r="AF18" s="75"/>
       <c r="AG18" s="75"/>
@@ -3517,7 +3477,7 @@
       <c r="AJ18" s="74"/>
       <c r="AK18" s="74"/>
       <c r="AL18" s="74"/>
-      <c r="AM18" s="107"/>
+      <c r="AM18" s="77"/>
       <c r="AN18" s="75"/>
       <c r="AO18" s="76"/>
       <c r="AP18" s="73"/>
@@ -3547,29 +3507,28 @@
         <v>301</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="49">
         <v>3</v>
       </c>
       <c r="D19" s="83">
-        <f>SUM(G19:BJ19)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E19" s="50"/>
       <c r="F19" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G19" s="53"/>
       <c r="H19" s="54"/>
-      <c r="I19" s="101"/>
+      <c r="I19" s="92"/>
       <c r="J19" s="55"/>
       <c r="K19" s="63"/>
       <c r="L19" s="57"/>
       <c r="M19" s="58"/>
       <c r="N19" s="53"/>
       <c r="O19" s="54"/>
-      <c r="P19" s="100"/>
+      <c r="P19" s="91"/>
       <c r="Q19" s="55"/>
       <c r="R19" s="56"/>
       <c r="S19" s="57"/>
@@ -3583,16 +3542,16 @@
       <c r="AA19" s="58"/>
       <c r="AB19" s="53"/>
       <c r="AC19" s="54"/>
-      <c r="AD19" s="103"/>
-      <c r="AE19" s="55"/>
-      <c r="AF19" s="56"/>
+      <c r="AD19" s="53"/>
+      <c r="AE19" s="53"/>
+      <c r="AF19" s="53"/>
       <c r="AG19" s="57"/>
       <c r="AH19" s="58"/>
       <c r="AI19" s="53"/>
       <c r="AJ19" s="54"/>
-      <c r="AK19" s="55"/>
-      <c r="AL19" s="55"/>
-      <c r="AM19" s="106"/>
+      <c r="AK19" s="53"/>
+      <c r="AL19" s="53"/>
+      <c r="AM19" s="53"/>
       <c r="AN19" s="57"/>
       <c r="AO19" s="58"/>
       <c r="AP19" s="53"/>
@@ -3622,14 +3581,13 @@
         <v>302</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="49">
         <v>5</v>
       </c>
       <c r="D20" s="83">
-        <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3644,9 +3602,9 @@
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
-      <c r="P20" s="99"/>
-      <c r="Q20" s="100"/>
-      <c r="R20" s="100"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="91"/>
+      <c r="R20" s="91"/>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
       <c r="U20" s="59"/>
@@ -3658,16 +3616,16 @@
       <c r="AA20" s="58"/>
       <c r="AB20" s="59"/>
       <c r="AC20" s="60"/>
-      <c r="AD20" s="103"/>
-      <c r="AE20" s="55"/>
-      <c r="AF20" s="56"/>
+      <c r="AD20" s="53"/>
+      <c r="AE20" s="53"/>
+      <c r="AF20" s="53"/>
       <c r="AG20" s="57"/>
       <c r="AH20" s="58"/>
       <c r="AI20" s="59"/>
       <c r="AJ20" s="60"/>
-      <c r="AK20" s="55"/>
-      <c r="AL20" s="55"/>
-      <c r="AM20" s="106"/>
+      <c r="AK20" s="53"/>
+      <c r="AL20" s="53"/>
+      <c r="AM20" s="53"/>
       <c r="AN20" s="57"/>
       <c r="AO20" s="58"/>
       <c r="AP20" s="59"/>
@@ -3703,8 +3661,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="83">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="50">
         <v>1</v>
@@ -3714,35 +3671,35 @@
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
-      <c r="K21" s="100"/>
+      <c r="K21" s="91"/>
       <c r="L21" s="57"/>
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
-      <c r="P21" s="98"/>
-      <c r="Q21" s="99"/>
-      <c r="R21" s="100"/>
+      <c r="P21" s="89"/>
+      <c r="Q21" s="90"/>
+      <c r="R21" s="91"/>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
       <c r="U21" s="59"/>
       <c r="V21" s="60"/>
-      <c r="W21" s="100"/>
+      <c r="W21" s="91"/>
       <c r="X21" s="55"/>
       <c r="Y21" s="56"/>
       <c r="Z21" s="57"/>
       <c r="AA21" s="58"/>
       <c r="AB21" s="59"/>
       <c r="AC21" s="60"/>
-      <c r="AD21" s="103"/>
-      <c r="AE21" s="55"/>
-      <c r="AF21" s="56"/>
+      <c r="AD21" s="53"/>
+      <c r="AE21" s="53"/>
+      <c r="AF21" s="53"/>
       <c r="AG21" s="57"/>
       <c r="AH21" s="58"/>
       <c r="AI21" s="59"/>
       <c r="AJ21" s="60"/>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="55"/>
-      <c r="AM21" s="106"/>
+      <c r="AK21" s="53"/>
+      <c r="AL21" s="53"/>
+      <c r="AM21" s="53"/>
       <c r="AN21" s="57"/>
       <c r="AO21" s="58"/>
       <c r="AP21" s="59"/>
@@ -3778,8 +3735,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="83">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E22" s="50">
         <v>1</v>
@@ -3794,30 +3750,30 @@
       <c r="M22" s="58"/>
       <c r="N22" s="59"/>
       <c r="O22" s="60"/>
-      <c r="P22" s="98"/>
-      <c r="Q22" s="99"/>
-      <c r="R22" s="99"/>
+      <c r="P22" s="91"/>
+      <c r="Q22" s="89"/>
+      <c r="R22" s="90"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
-      <c r="W22" s="100"/>
-      <c r="X22" s="100"/>
-      <c r="Y22" s="100"/>
+      <c r="W22" s="91"/>
+      <c r="X22" s="91"/>
+      <c r="Y22" s="91"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
       <c r="AB22" s="59"/>
       <c r="AC22" s="60"/>
-      <c r="AD22" s="103"/>
-      <c r="AE22" s="55"/>
-      <c r="AF22" s="56"/>
+      <c r="AD22" s="53"/>
+      <c r="AE22" s="53"/>
+      <c r="AF22" s="53"/>
       <c r="AG22" s="57"/>
       <c r="AH22" s="58"/>
       <c r="AI22" s="59"/>
       <c r="AJ22" s="60"/>
-      <c r="AK22" s="55"/>
-      <c r="AL22" s="55"/>
-      <c r="AM22" s="106"/>
+      <c r="AK22" s="53"/>
+      <c r="AL22" s="53"/>
+      <c r="AM22" s="53"/>
       <c r="AN22" s="57"/>
       <c r="AO22" s="58"/>
       <c r="AP22" s="59"/>
@@ -3853,7 +3809,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="83">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D20:D30" si="0">SUM(G23:BJ23)</f>
         <v>0</v>
       </c>
       <c r="E23" s="50">
@@ -3870,29 +3826,29 @@
       <c r="N23" s="59"/>
       <c r="O23" s="60"/>
       <c r="P23" s="61"/>
-      <c r="Q23" s="98"/>
-      <c r="R23" s="86"/>
+      <c r="Q23" s="89"/>
+      <c r="R23" s="89"/>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="100"/>
-      <c r="X23" s="108"/>
-      <c r="Y23" s="100"/>
+      <c r="W23" s="86"/>
+      <c r="X23" s="91"/>
+      <c r="Y23" s="91"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
       <c r="AB23" s="59"/>
       <c r="AC23" s="60"/>
-      <c r="AD23" s="105"/>
-      <c r="AE23" s="61"/>
-      <c r="AF23" s="56"/>
+      <c r="AD23" s="53"/>
+      <c r="AE23" s="53"/>
+      <c r="AF23" s="53"/>
       <c r="AG23" s="57"/>
       <c r="AH23" s="58"/>
       <c r="AI23" s="59"/>
       <c r="AJ23" s="60"/>
-      <c r="AK23" s="61"/>
-      <c r="AL23" s="61"/>
-      <c r="AM23" s="106"/>
+      <c r="AK23" s="53"/>
+      <c r="AL23" s="53"/>
+      <c r="AM23" s="53"/>
       <c r="AN23" s="57"/>
       <c r="AO23" s="58"/>
       <c r="AP23" s="59"/>
@@ -3945,29 +3901,29 @@
       <c r="N24" s="59"/>
       <c r="O24" s="60"/>
       <c r="P24" s="55"/>
-      <c r="Q24" s="98"/>
-      <c r="R24" s="98"/>
+      <c r="Q24" s="91"/>
+      <c r="R24" s="89"/>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
-      <c r="W24" s="100"/>
-      <c r="X24" s="100"/>
-      <c r="Y24" s="100"/>
+      <c r="W24" s="89"/>
+      <c r="X24" s="91"/>
+      <c r="Y24" s="91"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
       <c r="AB24" s="59"/>
       <c r="AC24" s="60"/>
-      <c r="AD24" s="105"/>
-      <c r="AE24" s="100"/>
-      <c r="AF24" s="100"/>
+      <c r="AD24" s="53"/>
+      <c r="AE24" s="53"/>
+      <c r="AF24" s="53"/>
       <c r="AG24" s="57"/>
       <c r="AH24" s="58"/>
       <c r="AI24" s="59"/>
       <c r="AJ24" s="60"/>
-      <c r="AK24" s="55"/>
-      <c r="AL24" s="55"/>
-      <c r="AM24" s="106"/>
+      <c r="AK24" s="53"/>
+      <c r="AL24" s="53"/>
+      <c r="AM24" s="53"/>
       <c r="AN24" s="57"/>
       <c r="AO24" s="58"/>
       <c r="AP24" s="59"/>
@@ -4026,23 +3982,23 @@
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
       <c r="V25" s="60"/>
-      <c r="W25" s="98"/>
-      <c r="X25" s="98"/>
-      <c r="Y25" s="100"/>
+      <c r="W25" s="89"/>
+      <c r="X25" s="89"/>
+      <c r="Y25" s="91"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
       <c r="AB25" s="59"/>
       <c r="AC25" s="60"/>
-      <c r="AD25" s="105"/>
-      <c r="AE25" s="100"/>
-      <c r="AF25" s="100"/>
+      <c r="AD25" s="53"/>
+      <c r="AE25" s="53"/>
+      <c r="AF25" s="53"/>
       <c r="AG25" s="57"/>
       <c r="AH25" s="58"/>
       <c r="AI25" s="59"/>
       <c r="AJ25" s="60"/>
-      <c r="AK25" s="100"/>
-      <c r="AL25" s="100"/>
-      <c r="AM25" s="106"/>
+      <c r="AK25" s="53"/>
+      <c r="AL25" s="53"/>
+      <c r="AM25" s="53"/>
       <c r="AN25" s="57"/>
       <c r="AO25" s="58"/>
       <c r="AP25" s="59"/>
@@ -4102,22 +4058,22 @@
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
       <c r="W26" s="55"/>
-      <c r="X26" s="98"/>
+      <c r="X26" s="89"/>
       <c r="Y26" s="56"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
       <c r="AB26" s="59"/>
       <c r="AC26" s="60"/>
-      <c r="AD26" s="103"/>
-      <c r="AE26" s="55"/>
-      <c r="AF26" s="100"/>
+      <c r="AD26" s="53"/>
+      <c r="AE26" s="53"/>
+      <c r="AF26" s="53"/>
       <c r="AG26" s="57"/>
       <c r="AH26" s="58"/>
       <c r="AI26" s="59"/>
       <c r="AJ26" s="60"/>
-      <c r="AK26" s="100"/>
-      <c r="AL26" s="100"/>
-      <c r="AM26" s="105"/>
+      <c r="AK26" s="53"/>
+      <c r="AL26" s="53"/>
+      <c r="AM26" s="53"/>
       <c r="AN26" s="57"/>
       <c r="AO26" s="58"/>
       <c r="AP26" s="59"/>
@@ -4150,7 +4106,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
@@ -4181,16 +4137,16 @@
       <c r="AA27" s="58"/>
       <c r="AB27" s="59"/>
       <c r="AC27" s="60"/>
-      <c r="AD27" s="103"/>
-      <c r="AE27" s="55"/>
-      <c r="AF27" s="56"/>
+      <c r="AD27" s="53"/>
+      <c r="AE27" s="53"/>
+      <c r="AF27" s="53"/>
       <c r="AG27" s="57"/>
       <c r="AH27" s="58"/>
       <c r="AI27" s="59"/>
       <c r="AJ27" s="60"/>
-      <c r="AK27" s="55"/>
-      <c r="AL27" s="55"/>
-      <c r="AM27" s="106"/>
+      <c r="AK27" s="53"/>
+      <c r="AL27" s="53"/>
+      <c r="AM27" s="53"/>
       <c r="AN27" s="57"/>
       <c r="AO27" s="58"/>
       <c r="AP27" s="59"/>
@@ -4252,16 +4208,16 @@
       <c r="AA28" s="58"/>
       <c r="AB28" s="59"/>
       <c r="AC28" s="60"/>
-      <c r="AD28" s="103"/>
-      <c r="AE28" s="55"/>
-      <c r="AF28" s="56"/>
+      <c r="AD28" s="53"/>
+      <c r="AE28" s="53"/>
+      <c r="AF28" s="53"/>
       <c r="AG28" s="57"/>
       <c r="AH28" s="58"/>
       <c r="AI28" s="59"/>
       <c r="AJ28" s="60"/>
-      <c r="AK28" s="55"/>
-      <c r="AL28" s="55"/>
-      <c r="AM28" s="106"/>
+      <c r="AK28" s="53"/>
+      <c r="AL28" s="53"/>
+      <c r="AM28" s="53"/>
       <c r="AN28" s="57"/>
       <c r="AO28" s="58"/>
       <c r="AP28" s="59"/>
@@ -4290,9 +4246,7 @@
       <c r="A29" s="12">
         <v>311</v>
       </c>
-      <c r="B29" s="46" t="s">
-        <v>32</v>
-      </c>
+      <c r="B29" s="46"/>
       <c r="C29" s="49"/>
       <c r="D29" s="83">
         <f t="shared" si="0"/>
@@ -4323,16 +4277,16 @@
       <c r="AA29" s="58"/>
       <c r="AB29" s="71"/>
       <c r="AC29" s="72"/>
-      <c r="AD29" s="103"/>
-      <c r="AE29" s="55"/>
-      <c r="AF29" s="56"/>
+      <c r="AD29" s="53"/>
+      <c r="AE29" s="53"/>
+      <c r="AF29" s="53"/>
       <c r="AG29" s="57"/>
       <c r="AH29" s="58"/>
       <c r="AI29" s="71"/>
       <c r="AJ29" s="72"/>
-      <c r="AK29" s="55"/>
-      <c r="AL29" s="55"/>
-      <c r="AM29" s="106"/>
+      <c r="AK29" s="53"/>
+      <c r="AL29" s="53"/>
+      <c r="AM29" s="53"/>
       <c r="AN29" s="57"/>
       <c r="AO29" s="58"/>
       <c r="AP29" s="71"/>
@@ -4392,16 +4346,16 @@
       <c r="AA30" s="58"/>
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
-      <c r="AD30" s="103"/>
-      <c r="AE30" s="55"/>
-      <c r="AF30" s="56"/>
+      <c r="AD30" s="53"/>
+      <c r="AE30" s="53"/>
+      <c r="AF30" s="53"/>
       <c r="AG30" s="57"/>
       <c r="AH30" s="58"/>
       <c r="AI30" s="69"/>
       <c r="AJ30" s="70"/>
-      <c r="AK30" s="55"/>
-      <c r="AL30" s="55"/>
-      <c r="AM30" s="106"/>
+      <c r="AK30" s="53"/>
+      <c r="AL30" s="53"/>
+      <c r="AM30" s="53"/>
       <c r="AN30" s="57"/>
       <c r="AO30" s="58"/>
       <c r="AP30" s="69"/>
@@ -4466,7 +4420,7 @@
       <c r="AA31" s="76"/>
       <c r="AB31" s="77"/>
       <c r="AC31" s="74"/>
-      <c r="AD31" s="104"/>
+      <c r="AD31" s="77"/>
       <c r="AE31" s="74"/>
       <c r="AF31" s="75"/>
       <c r="AG31" s="75"/>
@@ -4475,7 +4429,7 @@
       <c r="AJ31" s="74"/>
       <c r="AK31" s="74"/>
       <c r="AL31" s="74"/>
-      <c r="AM31" s="107"/>
+      <c r="AM31" s="77"/>
       <c r="AN31" s="75"/>
       <c r="AO31" s="76"/>
       <c r="AP31" s="73"/>
@@ -4505,7 +4459,7 @@
         <v>401</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="49">
         <v>2</v>
@@ -4536,21 +4490,21 @@
       <c r="V32" s="54"/>
       <c r="W32" s="55"/>
       <c r="X32" s="55"/>
-      <c r="Y32" s="98"/>
+      <c r="Y32" s="89"/>
       <c r="Z32" s="57"/>
       <c r="AA32" s="58"/>
       <c r="AB32" s="53"/>
       <c r="AC32" s="54"/>
-      <c r="AD32" s="103"/>
-      <c r="AE32" s="55"/>
-      <c r="AF32" s="56"/>
+      <c r="AD32" s="54"/>
+      <c r="AE32" s="54"/>
+      <c r="AF32" s="54"/>
       <c r="AG32" s="57"/>
       <c r="AH32" s="58"/>
       <c r="AI32" s="53"/>
       <c r="AJ32" s="54"/>
-      <c r="AK32" s="55"/>
-      <c r="AL32" s="55"/>
-      <c r="AM32" s="105"/>
+      <c r="AK32" s="54"/>
+      <c r="AL32" s="54"/>
+      <c r="AM32" s="54"/>
       <c r="AN32" s="57"/>
       <c r="AO32" s="58"/>
       <c r="AP32" s="53"/>
@@ -4580,7 +4534,7 @@
         <v>402</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="49">
         <v>2</v>
@@ -4611,26 +4565,26 @@
       <c r="V33" s="60"/>
       <c r="W33" s="55"/>
       <c r="X33" s="55"/>
-      <c r="Y33" s="98"/>
+      <c r="Y33" s="89"/>
       <c r="Z33" s="57"/>
       <c r="AA33" s="58"/>
       <c r="AB33" s="59"/>
       <c r="AC33" s="60"/>
-      <c r="AD33" s="103"/>
-      <c r="AE33" s="55"/>
-      <c r="AF33" s="56"/>
+      <c r="AD33" s="54"/>
+      <c r="AE33" s="54"/>
+      <c r="AF33" s="54"/>
       <c r="AG33" s="57"/>
       <c r="AH33" s="58"/>
       <c r="AI33" s="59"/>
       <c r="AJ33" s="60"/>
-      <c r="AK33" s="55"/>
-      <c r="AL33" s="55"/>
-      <c r="AM33" s="105"/>
+      <c r="AK33" s="54"/>
+      <c r="AL33" s="54"/>
+      <c r="AM33" s="54"/>
       <c r="AN33" s="57"/>
       <c r="AO33" s="58"/>
       <c r="AP33" s="59"/>
       <c r="AQ33" s="60"/>
-      <c r="AR33" s="100"/>
+      <c r="AR33" s="91"/>
       <c r="AS33" s="55"/>
       <c r="AT33" s="56"/>
       <c r="AU33" s="57"/>
@@ -4655,10 +4609,10 @@
         <v>403</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="83">
         <f t="shared" si="1"/>
@@ -4686,26 +4640,26 @@
       <c r="V34" s="60"/>
       <c r="W34" s="55"/>
       <c r="X34" s="55"/>
-      <c r="Y34" s="98"/>
+      <c r="Y34" s="89"/>
       <c r="Z34" s="57"/>
       <c r="AA34" s="58"/>
       <c r="AB34" s="59"/>
       <c r="AC34" s="60"/>
-      <c r="AD34" s="103"/>
-      <c r="AE34" s="55"/>
-      <c r="AF34" s="56"/>
+      <c r="AD34" s="54"/>
+      <c r="AE34" s="54"/>
+      <c r="AF34" s="54"/>
       <c r="AG34" s="57"/>
       <c r="AH34" s="58"/>
       <c r="AI34" s="59"/>
       <c r="AJ34" s="60"/>
-      <c r="AK34" s="55"/>
-      <c r="AL34" s="55"/>
-      <c r="AM34" s="105"/>
+      <c r="AK34" s="54"/>
+      <c r="AL34" s="54"/>
+      <c r="AM34" s="54"/>
       <c r="AN34" s="57"/>
       <c r="AO34" s="58"/>
       <c r="AP34" s="59"/>
       <c r="AQ34" s="60"/>
-      <c r="AR34" s="98"/>
+      <c r="AR34" s="89"/>
       <c r="AS34" s="55"/>
       <c r="AT34" s="56"/>
       <c r="AU34" s="57"/>
@@ -4760,16 +4714,16 @@
       <c r="AA35" s="58"/>
       <c r="AB35" s="69"/>
       <c r="AC35" s="70"/>
-      <c r="AD35" s="103"/>
-      <c r="AE35" s="55"/>
-      <c r="AF35" s="56"/>
+      <c r="AD35" s="54"/>
+      <c r="AE35" s="54"/>
+      <c r="AF35" s="54"/>
       <c r="AG35" s="57"/>
       <c r="AH35" s="58"/>
       <c r="AI35" s="69"/>
       <c r="AJ35" s="70"/>
-      <c r="AK35" s="55"/>
-      <c r="AL35" s="55"/>
-      <c r="AM35" s="106"/>
+      <c r="AK35" s="54"/>
+      <c r="AL35" s="54"/>
+      <c r="AM35" s="54"/>
       <c r="AN35" s="57"/>
       <c r="AO35" s="58"/>
       <c r="AP35" s="69"/>
@@ -4807,7 +4761,7 @@
       </c>
       <c r="D36" s="42">
         <f>SUM(D37:D38)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E36" s="32"/>
       <c r="F36" s="31"/>
@@ -4873,14 +4827,14 @@
         <v>501</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="49">
         <v>10</v>
       </c>
       <c r="D37" s="83">
         <f>SUM(G37:BJ37)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E37" s="50"/>
       <c r="F37" s="51"/>
@@ -4908,15 +4862,23 @@
       <c r="AB37" s="53"/>
       <c r="AC37" s="54"/>
       <c r="AD37" s="55"/>
-      <c r="AE37" s="55"/>
-      <c r="AF37" s="56"/>
+      <c r="AE37" s="89">
+        <v>2</v>
+      </c>
+      <c r="AF37" s="89">
+        <v>2</v>
+      </c>
       <c r="AG37" s="57"/>
       <c r="AH37" s="58"/>
       <c r="AI37" s="53"/>
       <c r="AJ37" s="54"/>
       <c r="AK37" s="55"/>
-      <c r="AL37" s="55"/>
-      <c r="AM37" s="56"/>
+      <c r="AL37" s="89">
+        <v>2</v>
+      </c>
+      <c r="AM37" s="89">
+        <v>2</v>
+      </c>
       <c r="AN37" s="57"/>
       <c r="AO37" s="58"/>
       <c r="AP37" s="53"/>
@@ -5089,7 +5051,7 @@
         <v>601</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" s="49"/>
       <c r="D40" s="83">
@@ -5160,7 +5122,7 @@
         <v>602</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="49"/>
       <c r="D41" s="83">
@@ -5306,7 +5268,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>7</v>
+        <v>34.5</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5328,7 +5290,7 @@
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5408,11 +5370,11 @@
       </c>
       <c r="AE43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG43" s="39">
         <f t="shared" si="3"/>
@@ -5436,11 +5398,11 @@
       </c>
       <c r="AL43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM43" s="39">
         <f t="shared" ref="AM43:BD43" si="4">SUM(AM9:AM42)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN43" s="39">
         <f t="shared" si="4"/>
@@ -5581,10 +5543,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1"/>
     <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="97"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5593,28 +5555,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1">
-      <c r="A3" s="94" t="str">
+      <c r="A3" s="98" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="95"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>4</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="18" thickTop="1" thickBot="1">
-      <c r="A4" s="94" t="str">
+      <c r="A4" s="98" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>11</v>
@@ -5627,28 +5589,28 @@
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="18" thickTop="1" thickBot="1">
-      <c r="A5" s="94" t="str">
+      <c r="A5" s="98" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="95"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>36</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="18" thickTop="1" thickBot="1">
-      <c r="A6" s="94" t="str">
+      <c r="A6" s="98" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="95"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>4</v>
@@ -5660,27 +5622,27 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="18" thickTop="1" thickBot="1">
-      <c r="A7" s="94" t="str">
+      <c r="A7" s="98" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>10</v>
       </c>
       <c r="D7" s="80">
         <f>Zeitplanung!D36</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickTop="1" thickBot="1">
-      <c r="A8" s="94" t="str">
+      <c r="A8" s="98" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="95"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
         <v>0</v>

</xml_diff>

<commit_message>
Push 13.12. ich habe mit 2d Array eingabefelder erstellt
</commit_message>
<xml_diff>
--- a/Zeitplanung SudoSolve.xlsx
+++ b/Zeitplanung SudoSolve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritzwicki/Sudo_Solve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598466AB-829B-9643-902D-7E0AA805D676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE8EDC7-C91D-5A40-AD53-7187EE2A1000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1663,7 +1663,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2170,8 +2170,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1"/>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3513,7 +3513,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" s="50"/>
       <c r="F19" s="51" t="s">
@@ -3523,7 +3523,9 @@
       <c r="H19" s="54"/>
       <c r="I19" s="92"/>
       <c r="J19" s="55"/>
-      <c r="K19" s="63"/>
+      <c r="K19" s="63">
+        <v>1</v>
+      </c>
       <c r="L19" s="57"/>
       <c r="M19" s="58"/>
       <c r="N19" s="53"/>
@@ -3597,12 +3599,16 @@
       <c r="H20" s="60"/>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
-      <c r="K20" s="63"/>
+      <c r="K20" s="63">
+        <v>7</v>
+      </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
-      <c r="P20" s="63"/>
+      <c r="P20" s="63">
+        <v>2</v>
+      </c>
       <c r="Q20" s="91"/>
       <c r="R20" s="91"/>
       <c r="S20" s="57"/>
@@ -3676,7 +3682,9 @@
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
-      <c r="P21" s="89"/>
+      <c r="P21" s="89">
+        <v>3</v>
+      </c>
       <c r="Q21" s="90"/>
       <c r="R21" s="91"/>
       <c r="S21" s="57"/>
@@ -3751,7 +3759,9 @@
       <c r="N22" s="59"/>
       <c r="O22" s="60"/>
       <c r="P22" s="91"/>
-      <c r="Q22" s="89"/>
+      <c r="Q22" s="89">
+        <v>4</v>
+      </c>
       <c r="R22" s="90"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
@@ -3809,8 +3819,8 @@
         <v>2</v>
       </c>
       <c r="D23" s="83">
-        <f t="shared" ref="D20:D30" si="0">SUM(G23:BJ23)</f>
-        <v>0</v>
+        <f t="shared" ref="D23:D30" si="0">SUM(G23:BJ23)</f>
+        <v>4</v>
       </c>
       <c r="E23" s="50">
         <v>1</v>
@@ -3826,7 +3836,9 @@
       <c r="N23" s="59"/>
       <c r="O23" s="60"/>
       <c r="P23" s="61"/>
-      <c r="Q23" s="89"/>
+      <c r="Q23" s="89">
+        <v>4</v>
+      </c>
       <c r="R23" s="89"/>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
@@ -5268,7 +5280,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>34.5</v>
+        <v>36.5</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5290,7 +5302,7 @@
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>12.5</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5310,11 +5322,11 @@
       </c>
       <c r="P43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
@@ -5600,7 +5612,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Push 20.12 Sudoku ausfüllen und Korrigieren funktioniert. Der SudokuSolver ist in Arbeit
</commit_message>
<xml_diff>
--- a/Zeitplanung SudoSolve.xlsx
+++ b/Zeitplanung SudoSolve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritzwicki/Sudo_Solve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D84B02F-EA56-F049-AA93-146C0238F805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F194CB24-16B9-8D4E-8086-2F574C81B304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="3700" windowWidth="33600" windowHeight="20540" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1663,7 +1663,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2171,7 +2171,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="AD27" sqref="AD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1"/>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>21</v>
+        <v>36.5</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3820,7 +3820,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" ref="D23:D30" si="0">SUM(G23:BJ23)</f>
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="E23" s="50">
         <v>1</v>
@@ -3840,13 +3840,15 @@
         <v>4</v>
       </c>
       <c r="R23" s="89">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="86"/>
+      <c r="W23" s="86">
+        <v>1.5</v>
+      </c>
       <c r="X23" s="91"/>
       <c r="Y23" s="91"/>
       <c r="Z23" s="57"/>
@@ -3899,7 +3901,7 @@
       </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E24" s="50">
         <v>1</v>
@@ -3917,14 +3919,18 @@
       <c r="P24" s="55"/>
       <c r="Q24" s="91"/>
       <c r="R24" s="89">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
-      <c r="W24" s="89"/>
-      <c r="X24" s="91"/>
+      <c r="W24" s="89">
+        <v>5</v>
+      </c>
+      <c r="X24" s="89">
+        <v>8</v>
+      </c>
       <c r="Y24" s="91"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
@@ -3998,9 +4004,9 @@
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
       <c r="V25" s="60"/>
-      <c r="W25" s="89"/>
-      <c r="X25" s="89"/>
-      <c r="Y25" s="91"/>
+      <c r="W25" s="55"/>
+      <c r="X25" s="55"/>
+      <c r="Y25" s="89"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
       <c r="AB25" s="59"/>
@@ -4074,7 +4080,7 @@
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
       <c r="W26" s="55"/>
-      <c r="X26" s="89"/>
+      <c r="X26" s="55"/>
       <c r="Y26" s="56"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
@@ -5284,7 +5290,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>40.5</v>
+        <v>56</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5334,7 +5340,7 @@
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S43" s="39">
         <f t="shared" si="3"/>
@@ -5354,11 +5360,11 @@
       </c>
       <c r="W43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y43" s="39">
         <f t="shared" si="3"/>
@@ -5616,7 +5622,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>21</v>
+        <v>36.5</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Push 20.12 Das Sudoku funktionier. Der Solver noch nicht
</commit_message>
<xml_diff>
--- a/Zeitplanung SudoSolve.xlsx
+++ b/Zeitplanung SudoSolve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritzwicki/Sudo_Solve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F194CB24-16B9-8D4E-8086-2F574C81B304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9744C7-42F5-7741-A857-F52F68A4E3F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1663,7 +1663,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.5</c:v>
+                  <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2171,7 +2171,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AD27" sqref="AD27"/>
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1"/>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>36.5</v>
+        <v>44.5</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E25" s="50">
         <v>2</v>
@@ -4006,7 +4006,9 @@
       <c r="V25" s="60"/>
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
-      <c r="Y25" s="89"/>
+      <c r="Y25" s="89">
+        <v>8</v>
+      </c>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
       <c r="AB25" s="59"/>
@@ -5290,7 +5292,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5368,7 +5370,7 @@
       </c>
       <c r="Y43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z43" s="39">
         <f t="shared" si="3"/>
@@ -5622,7 +5624,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>36.5</v>
+        <v>44.5</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>